<commit_message>
update RMD, knit to html. show results of coho controls
</commit_message>
<xml_diff>
--- a/Hypotheses to test.xlsx
+++ b/Hypotheses to test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/thomas_buehrens_dfw_wa_gov/Documents/Documents/WDFW Fish Management/CRSSE/Cowlitz HM/Study Implementation/reports/final contract deliverables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/thomas_buehrens_dfw_wa_gov/Documents/Documents/Scripts/Hooking_Mortality/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="8_{C349AF92-AE87-4A26-8011-9AE0A1618DBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{353C6BD2-ED01-4167-9093-2A95DB059A6F}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="8_{C349AF92-AE87-4A26-8011-9AE0A1618DBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{57DA69EC-CAE0-48B5-B0C5-E8B6D80C1B0D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E603068E-021F-422C-B6B8-2364EEC59CAE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="84">
   <si>
     <t>Hypothesis</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>salmon vs steelhead models</t>
+  </si>
+  <si>
+    <t>Interaction between T/C and location because treatment effect "more fully expressed" for fish that take longer to be recaptured</t>
   </si>
 </sst>
 </file>
@@ -736,11 +739,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63FE60E1-65D0-4B45-B8C0-65AF8CA4680B}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -862,38 +865,36 @@
       <c r="E8" s="8"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" customFormat="1" ht="28" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="10"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" customFormat="1" ht="28" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="10"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -905,362 +906,405 @@
         <v>32</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="D12" s="6"/>
       <c r="E12" s="8"/>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="8"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="8"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="D16" s="6"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="3" t="s">
-        <v>59</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" customFormat="1" ht="28" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="8"/>
+        <v>63</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="10"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" customFormat="1" ht="28" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="8"/>
+        <v>63</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="10"/>
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="8"/>
+        <v>63</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="10"/>
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="8"/>
+        <v>63</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="10"/>
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="8"/>
+        <v>63</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="10"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" customFormat="1" ht="28" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" customFormat="1" ht="28" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" customFormat="1" ht="28" x14ac:dyDescent="0.35">
+      <c r="B25" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="B26" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="5"/>
       <c r="D26" s="6"/>
       <c r="E26" s="8"/>
-      <c r="F26" s="3"/>
+      <c r="F26" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>47</v>
+      <c r="B27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B28" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>52</v>
-      </c>
+      <c r="B30" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="8"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="B31" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="8"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B32" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B33" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B34" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B35" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F26">
-    <sortCondition ref="A2:A26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F46">
+    <sortCondition ref="A2:A46"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>